<commit_message>
WIP uploads show before
</commit_message>
<xml_diff>
--- a/public/files/example-employees-csv.xlsx
+++ b/public/files/example-employees-csv.xlsx
@@ -28,19 +28,19 @@
     <t xml:space="preserve">Roles</t>
   </si>
   <si>
-    <t xml:space="preserve">Reporting Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reporting Manager Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Department Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location Office Name</t>
+    <t xml:space="preserve">ReportingManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReportingManagerEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepartmentName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContactNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationOfficeName</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
@@ -135,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -170,17 +170,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,14 +240,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -291,7 +272,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.26"/>
@@ -392,13 +373,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -430,7 +411,7 @@
       <c r="C5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="0" t="s">

</xml_diff>

<commit_message>
WIP validation (upload employee)
</commit_message>
<xml_diff>
--- a/public/files/example-employees-csv.xlsx
+++ b/public/files/example-employees-csv.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">shumonsb@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana</t>
+    <t xml:space="preserve">Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhaka Office</t>
   </si>
   <si>
     <t xml:space="preserve">employee@gmail.com</t>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">itely</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employee4@mail.cm</t>
   </si>
 </sst>
 </file>
@@ -263,7 +260,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,7 +424,7 @@
         <v>123456</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -438,7 +435,7 @@
     <hyperlink ref="D4" r:id="rId4" display="mono@gmail.com"/>
     <hyperlink ref="I4" r:id="rId5" display="employee3@mail.com"/>
     <hyperlink ref="D5" r:id="rId6" display="sb2@gmail.com"/>
-    <hyperlink ref="I5" r:id="rId7" display="employee4@mail.cm"/>
+    <hyperlink ref="I5" r:id="rId7" display="shumonsb@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
completed employee upload logic
</commit_message>
<xml_diff>
--- a/public/files/example-employees-csv.xlsx
+++ b/public/files/example-employees-csv.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">Roles</t>
   </si>
   <si>
-    <t xml:space="preserve">ReportingManager</t>
-  </si>
-  <si>
     <t xml:space="preserve">ReportingManagerEmail</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t xml:space="preserve">admin</t>
   </si>
   <si>
-    <t xml:space="preserve">shumon babu</t>
-  </si>
-  <si>
     <t xml:space="preserve">shumonsb@gmail.com</t>
   </si>
   <si>
@@ -82,7 +76,7 @@
     <t xml:space="preserve">business</t>
   </si>
   <si>
-    <t xml:space="preserve">Dhaka</t>
+    <t xml:space="preserve">Chicago Office</t>
   </si>
   <si>
     <t xml:space="preserve">example@email.com</t>
@@ -91,37 +85,16 @@
     <t xml:space="preserve">mono ranjan 3</t>
   </si>
   <si>
-    <t xml:space="preserve">mono ranjan 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">mono@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Dep 2</t>
   </si>
   <si>
-    <t xml:space="preserve">london</t>
+    <t xml:space="preserve">London Office</t>
   </si>
   <si>
     <t xml:space="preserve">employee3@mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shumon babu 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sb2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itely</t>
   </si>
 </sst>
 </file>
@@ -132,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -162,11 +135,28 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,15 +210,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,7 +238,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,17 +262,17 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.04"/>
@@ -285,157 +287,124 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="n">
+        <v>9641234</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="7" t="n">
+        <v>123456</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>9641234</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>123456</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="5" t="n">
+        <v>8976543</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="n">
+        <v>123456</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="n">
-        <v>8976543</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>123456</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="E4" s="7" t="n">
+        <v>4356434</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" s="7" t="n">
+        <v>123456</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>4356434</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>5675676</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="shumonsb@gmail.com"/>
-    <hyperlink ref="I2" r:id="rId2" display="employee@gmail.com"/>
-    <hyperlink ref="I3" r:id="rId3" display="example@email.com"/>
-    <hyperlink ref="D4" r:id="rId4" display="mono@gmail.com"/>
-    <hyperlink ref="I4" r:id="rId5" display="employee3@mail.com"/>
-    <hyperlink ref="D5" r:id="rId6" display="sb2@gmail.com"/>
-    <hyperlink ref="I5" r:id="rId7" display="shumonsb@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="shumonsb@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId2" display="employee@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="example2@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId4" display="example@email.com"/>
+    <hyperlink ref="C4" r:id="rId5" display="mono@gmail.com"/>
+    <hyperlink ref="H4" r:id="rId6" display="employee3@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>